<commit_message>
add database-diagram-20141015.jpg, add ProjectOverview.docx
</commit_message>
<xml_diff>
--- a/Document/Task.xlsx
+++ b/Document/Task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Nguyễn Ngọc Thanh Hải</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>done</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -436,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -462,6 +459,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -522,8 +521,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,89 +867,93 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -953,98 +966,102 @@
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="16" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="41" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17" t="s">
+      <c r="E17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="18" t="s">
@@ -1057,55 +1074,57 @@
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="44" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -1127,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,10 +1178,10 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="48" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1203,10 +1222,10 @@
       <c r="B4" s="3">
         <v>14</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="47">
         <v>15</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="48">
         <v>16</v>
       </c>
       <c r="E4" s="4">
@@ -1269,26 +1288,26 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="37" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="32">
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1300,8 +1319,8 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1313,14 +1332,14 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="36"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="9"/>

</xml_diff>

<commit_message>
update Task.xlsx, add ClassDiagram
</commit_message>
<xml_diff>
--- a/Document/Task.xlsx
+++ b/Document/Task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Nguyễn Ngọc Thanh Hải</t>
   </si>
@@ -121,6 +121,33 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Web Interface</t>
+  </si>
+  <si>
+    <t>Web js game</t>
+  </si>
+  <si>
+    <t>23h 20/10/2014</t>
+  </si>
+  <si>
+    <t>23h 21/10/2014</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Code BLL</t>
+  </si>
+  <si>
+    <t>Code Dal</t>
+  </si>
+  <si>
+    <t>23h 22/10/2014</t>
+  </si>
+  <si>
+    <t>Code Servlet</t>
   </si>
 </sst>
 </file>
@@ -433,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -461,66 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,6 +500,68 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +896,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -884,7 +913,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="19" t="s">
         <v>23</v>
       </c>
@@ -897,7 +926,7 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="19" t="s">
         <v>24</v>
       </c>
@@ -910,7 +939,7 @@
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="19" t="s">
         <v>31</v>
       </c>
@@ -925,206 +954,230 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-      <c r="C13" s="41" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
-      <c r="C25" s="44" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="30"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="30"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="30"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -1146,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,16 +1231,16 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1222,16 +1275,16 @@
       <c r="B4" s="3">
         <v>14</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="27">
         <v>15</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="27">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="27">
         <v>17</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="28">
         <v>18</v>
       </c>
       <c r="G4" s="4">
@@ -1288,29 +1341,29 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="39" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="40"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="34">
+      <c r="B10" s="42">
         <v>1</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1319,10 +1372,10 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1332,14 +1385,14 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="9"/>

</xml_diff>